<commit_message>
Signed-off-by: Rafael Souza <rafael45m@gmail.com>
</commit_message>
<xml_diff>
--- a/Documentação Gerencia de Risco/Documentação Gerência de Risco.xlsx
+++ b/Documentação Gerencia de Risco/Documentação Gerência de Risco.xlsx
@@ -138,12 +138,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -152,29 +167,29 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,7 +488,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,231 +503,231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="31.5" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="8">
         <v>0.25</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="7">
         <v>8</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45">
-      <c r="A4" s="7">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="8">
         <v>0.5</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="7">
         <v>9</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="8">
         <v>0.5</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="45">
-      <c r="A6" s="7">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="8">
         <v>1</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="7">
         <v>3</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="75">
-      <c r="A7" s="7">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="8">
         <v>0.2</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="7">
         <v>8</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" spans="3:8">
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row r="18" spans="3:8">
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="3:8">
-      <c r="C19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>